<commit_message>
updated code and input data
</commit_message>
<xml_diff>
--- a/Input/TTFdata.xlsx
+++ b/Input/TTFdata.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veraisice/Desktop/Comodity-Market-Research/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF086B9E-82B3-9F48-9E43-C49435B785E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CA3656-9C05-884A-9380-1FF2633F5199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2560" windowWidth="25600" windowHeight="11180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="option prices" sheetId="2" r:id="rId1"/>
     <sheet name="August" sheetId="4" r:id="rId2"/>
-    <sheet name="September" sheetId="5" r:id="rId3"/>
-    <sheet name="Futures" sheetId="6" r:id="rId4"/>
+    <sheet name="September" sheetId="9" r:id="rId3"/>
+    <sheet name="Sep" sheetId="5" r:id="rId4"/>
+    <sheet name="Futures" sheetId="6" r:id="rId5"/>
+    <sheet name="October" sheetId="10" r:id="rId6"/>
+    <sheet name="November" sheetId="11" r:id="rId7"/>
+    <sheet name="December" sheetId="12" r:id="rId8"/>
+    <sheet name="January" sheetId="13" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="Time_To_Maturity" localSheetId="2">#REF!</definedName>
     <definedName name="Time_To_Maturity">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="14">
   <si>
     <t>Today</t>
   </si>
@@ -50,16 +56,7 @@
     <t>1-Month Future</t>
   </si>
   <si>
-    <t>AUG</t>
-  </si>
-  <si>
     <t>Calls</t>
-  </si>
-  <si>
-    <t>SEP</t>
-  </si>
-  <si>
-    <t>OCT</t>
   </si>
   <si>
     <t>NOV</t>
@@ -96,10 +93,24 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF25323C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,13 +154,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30:N50"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="N128" sqref="N128:O128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -443,62 +459,67 @@
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44005</v>
+        <v>44004</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L3" t="s">
-        <v>3</v>
+      <c r="L3" s="9">
+        <v>44044</v>
       </c>
       <c r="M3" s="5">
         <v>44037</v>
       </c>
       <c r="N3">
-        <v>8.7671232876712329E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="1">
-        <v>44013</v>
+        <f>(M3-A2)/252</f>
+        <v>0.13095238095238096</v>
+      </c>
+      <c r="O3">
+        <f>(M3-A2)/365</f>
+        <v>9.0410958904109592E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="5">
+        <v>44007</v>
       </c>
       <c r="C4">
         <v>5.4950000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
-        <v>44044</v>
+        <v>44037</v>
       </c>
       <c r="C6">
         <v>5.8049999999999997</v>
       </c>
       <c r="L6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="L7">
         <v>4</v>
@@ -510,15 +531,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
-        <v>44075</v>
+        <v>44072</v>
       </c>
       <c r="C8">
         <v>6.49</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="L9">
         <v>4.5</v>
@@ -530,15 +551,15 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
-        <v>44105</v>
+        <v>44103</v>
       </c>
       <c r="C10">
         <v>8.1850000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="L11">
         <v>5</v>
@@ -550,7 +571,7 @@
         <v>0.38500000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>44136</v>
       </c>
@@ -558,7 +579,7 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="L13">
         <v>5.5</v>
@@ -570,7 +591,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
         <v>44166</v>
       </c>
@@ -578,7 +599,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="L15">
         <v>6</v>
@@ -590,7 +611,7 @@
         <v>0.82499999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
         <v>44197</v>
       </c>
@@ -598,7 +619,7 @@
         <v>12.41</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="L17">
         <v>6.5</v>
@@ -610,7 +631,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="5">
         <v>44228</v>
       </c>
@@ -618,7 +639,7 @@
         <v>12.414999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="L19">
         <v>7</v>
@@ -630,7 +651,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="5">
         <v>44256</v>
       </c>
@@ -638,7 +659,7 @@
         <v>12.244999999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="L21">
         <v>7.5</v>
@@ -650,7 +671,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="5">
         <v>44287</v>
       </c>
@@ -658,7 +679,7 @@
         <v>11.795</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="L23">
         <v>8</v>
@@ -670,7 +691,7 @@
         <v>2.29</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="5">
         <v>44317</v>
       </c>
@@ -678,7 +699,7 @@
         <v>11.52</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="L25">
         <v>8.5</v>
@@ -690,7 +711,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="5">
         <v>44348</v>
       </c>
@@ -698,30 +719,35 @@
         <v>11.34</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="5">
         <v>44378</v>
       </c>
       <c r="C28">
         <v>11.24</v>
       </c>
-      <c r="L28" t="s">
-        <v>5</v>
+      <c r="L28" s="9">
+        <v>44075</v>
       </c>
       <c r="M28" s="5">
         <v>44068</v>
       </c>
       <c r="N28">
-        <v>0.17260273972602741</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+        <f>(M28-A2)/252</f>
+        <v>0.25396825396825395</v>
+      </c>
+      <c r="O28">
+        <f>(M28-A2)/365</f>
+        <v>0.17534246575342466</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="5">
         <v>44409</v>
       </c>
@@ -729,19 +755,19 @@
         <v>11.38</v>
       </c>
       <c r="L30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="5">
         <v>44440</v>
       </c>
@@ -918,10 +944,10 @@
         <v>1.9750000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="5"/>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="5">
         <v>44713</v>
       </c>
@@ -938,10 +964,10 @@
         <v>2.355</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="5"/>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="5">
         <v>44743</v>
       </c>
@@ -949,19 +975,24 @@
         <v>13.234999999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="5"/>
-      <c r="L53" t="s">
-        <v>6</v>
+      <c r="L53" s="9">
+        <v>44105</v>
       </c>
       <c r="M53" s="5">
-        <v>44099</v>
+        <v>44103</v>
       </c>
       <c r="N53">
-        <v>0.25753424657534246</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+        <f>(M53-A2)/252</f>
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="O53">
+        <f>(M53-A2)/252</f>
+        <v>0.39285714285714285</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B54" s="5">
         <v>44774</v>
       </c>
@@ -969,19 +1000,19 @@
         <v>13.404999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" s="5"/>
       <c r="L55" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M55" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B56" s="5">
         <v>44805</v>
       </c>
@@ -989,7 +1020,7 @@
         <v>13.435</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="5"/>
       <c r="L57">
         <v>6</v>
@@ -1001,7 +1032,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B58" s="5">
         <v>44835</v>
       </c>
@@ -1009,7 +1040,7 @@
         <v>14.71</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B59" s="5"/>
       <c r="L59">
         <v>6.5</v>
@@ -1021,7 +1052,7 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B60" s="5">
         <v>44866</v>
       </c>
@@ -1029,7 +1060,7 @@
         <v>15.065</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B61" s="5"/>
       <c r="L61">
         <v>7</v>
@@ -1041,7 +1072,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B62" s="5">
         <v>44896</v>
       </c>
@@ -1049,7 +1080,7 @@
         <v>15.695</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B63" s="5"/>
       <c r="L63">
         <v>7.5</v>
@@ -1061,7 +1092,7 @@
         <v>0.89500000000000002</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B64" s="5">
         <v>44927</v>
       </c>
@@ -1069,7 +1100,7 @@
         <v>16.045000000000002</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B65" s="5"/>
       <c r="L65">
         <v>8</v>
@@ -1081,7 +1112,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B66" s="5">
         <v>44958</v>
       </c>
@@ -1089,7 +1120,7 @@
         <v>15.904999999999999</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B67" s="5"/>
       <c r="L67">
         <v>8.5</v>
@@ -1101,7 +1132,7 @@
         <v>1.395</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B68" s="5">
         <v>44986</v>
       </c>
@@ -1109,7 +1140,7 @@
         <v>15.675000000000001</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B69" s="5"/>
       <c r="L69">
         <v>9</v>
@@ -1121,7 +1152,7 @@
         <v>1.6950000000000001</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B70" s="5">
         <v>45017</v>
       </c>
@@ -1129,7 +1160,7 @@
         <v>14.565</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B71" s="5"/>
       <c r="L71">
         <v>9.5</v>
@@ -1141,7 +1172,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B72" s="5">
         <v>45047</v>
       </c>
@@ -1149,7 +1180,7 @@
         <v>14.01</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B73" s="5"/>
       <c r="L73">
         <v>10</v>
@@ -1161,7 +1192,7 @@
         <v>2.39</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="5">
         <v>45078</v>
       </c>
@@ -1169,7 +1200,7 @@
         <v>13.52</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B75" s="5"/>
       <c r="L75">
         <v>10.5</v>
@@ -1181,7 +1212,7 @@
         <v>2.7749999999999999</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B76" s="5">
         <v>45108</v>
       </c>
@@ -1189,10 +1220,10 @@
         <v>13.234999999999999</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B77" s="5"/>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B78" s="5">
         <v>45139</v>
       </c>
@@ -1200,19 +1231,24 @@
         <v>13.7</v>
       </c>
       <c r="L78" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M78" s="5">
-        <v>44129</v>
+        <v>44133</v>
       </c>
       <c r="N78">
-        <v>0.33972602739726027</v>
-      </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
+        <f>(M78-A2)/252</f>
+        <v>0.51190476190476186</v>
+      </c>
+      <c r="O78">
+        <f>C12</f>
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B80" s="5">
         <v>45170</v>
       </c>
@@ -1220,13 +1256,13 @@
         <v>14.25</v>
       </c>
       <c r="L80" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M80" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="N80" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="2:19" x14ac:dyDescent="0.2">
@@ -1473,13 +1509,18 @@
     <row r="103" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B103" s="5"/>
       <c r="L103" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M103" s="5">
-        <v>44160</v>
+        <v>44162</v>
       </c>
       <c r="N103">
-        <v>0.42465753424657532</v>
+        <f>(M103-A2)/252</f>
+        <v>0.62698412698412698</v>
+      </c>
+      <c r="O103">
+        <f>C14</f>
+        <v>12.09</v>
       </c>
     </row>
     <row r="104" spans="2:19" x14ac:dyDescent="0.2">
@@ -1490,19 +1531,19 @@
         <v>14.56</v>
       </c>
       <c r="L104" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B105" s="5"/>
       <c r="L105" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M105" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N105" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="2:19" x14ac:dyDescent="0.2">
@@ -1754,19 +1795,24 @@
         <v>14.44</v>
       </c>
       <c r="L128" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M128" s="5">
-        <v>44190</v>
+        <v>44195</v>
       </c>
       <c r="N128">
-        <v>0.50684931506849318</v>
+        <f>(M128-A2)/252</f>
+        <v>0.75793650793650791</v>
+      </c>
+      <c r="O128">
+        <f>C16</f>
+        <v>12.41</v>
       </c>
     </row>
     <row r="129" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B129" s="5"/>
       <c r="L129" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.2">
@@ -1777,13 +1823,13 @@
         <v>15.494999999999999</v>
       </c>
       <c r="L130" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M130" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N130" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="131" spans="2:19" x14ac:dyDescent="0.2">
@@ -1954,7 +2000,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1964,16 +2010,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1983,29 +2029,28 @@
       <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1.9450000000000001</v>
       </c>
-      <c r="C2">
-        <v>0.14000000000000001</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2">
-        <v>0.12698412698412698</v>
+        <f>'option prices'!N3</f>
+        <v>0.13095238095238096</v>
       </c>
       <c r="E2">
-        <v>5.4950000000000001</v>
+        <f>'option prices'!C6</f>
+        <v>5.8049999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4.5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>1.5449999999999999</v>
       </c>
-      <c r="C3">
-        <v>0.24</v>
-      </c>
+      <c r="C3" s="4"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -2101,29 +2146,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CC5807-2312-904F-A997-63E8E6E81D9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFBF821-BD85-B94B-A1EF-F21E7ED9DD1F}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2134,14 +2179,13 @@
       <c r="B2">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>0.20499999999999999</v>
-      </c>
       <c r="D2">
-        <v>0.25</v>
+        <f>'option prices'!N28</f>
+        <v>0.25396825396825395</v>
       </c>
       <c r="E2">
-        <v>5.8049999999999997</v>
+        <f>'option prices'!C8</f>
+        <v>6.49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2151,9 +2195,7 @@
       <c r="B3">
         <v>4.5</v>
       </c>
-      <c r="C3">
-        <v>0.31</v>
-      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -2249,10 +2291,624 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CC5807-2312-904F-A997-63E8E6E81D9A}">
+  <dimension ref="A1:F128"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <f>6.81</f>
+        <v>6.81</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.25</v>
+      </c>
+      <c r="E2">
+        <v>5.8049999999999997</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>6.31</v>
+      </c>
+      <c r="B3">
+        <f>$B2+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.31</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>5.81</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B24" si="0">$B3+0.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>0.44</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>5.31</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0.6</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>3.81</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="C8">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <f>3.315-0.63</f>
+        <v>2.6850000000000001</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1.625</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>2.82</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="C10">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>2.33</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>2.355</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>1.85</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>11.5</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="8"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="8"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="8"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="8"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="8"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="8"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="8"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="8"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="8"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="8"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="8"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="8"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="8"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="8"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="8"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="8"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="8"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="8"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="8"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="8"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="8"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="8"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="8"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="8"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="8"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="8"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="8"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="8"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="8"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="8"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="8"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="8"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="8"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="8"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="8"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="8"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="8"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="8"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="8"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="8"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="8"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="8"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="8"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="8"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="8"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="8"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="8"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="8"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" s="8"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="8"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" s="8"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" s="8"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" s="8"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90C419A-A780-2A4C-B7E3-60000DB4F5CC}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2264,7 +2920,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2991,6 +3647,570 @@
       </c>
       <c r="C67">
         <v>7.9801587301587302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2A30BE-D971-A646-81A0-BDC983FC7870}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>2.56</v>
+      </c>
+      <c r="D2">
+        <f>'option prices'!N53</f>
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="E2">
+        <f>'option prices'!C10</f>
+        <v>8.1850000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6.5</v>
+      </c>
+      <c r="B3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7.5</v>
+      </c>
+      <c r="B5">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1.3149999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8.5</v>
+      </c>
+      <c r="B7">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9.5</v>
+      </c>
+      <c r="B9">
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10.5</v>
+      </c>
+      <c r="B11">
+        <v>0.46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C7D119-D262-DB40-8F24-48DC80CFE91A}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2.5649999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.51190476190476186</v>
+      </c>
+      <c r="E2">
+        <v>11.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>9.5</v>
+      </c>
+      <c r="B3">
+        <v>2.2349999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1.93</v>
+      </c>
+      <c r="C4">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10.5</v>
+      </c>
+      <c r="B5">
+        <v>1.66</v>
+      </c>
+      <c r="C5">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>1.415</v>
+      </c>
+      <c r="C6">
+        <v>1.365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>11.5</v>
+      </c>
+      <c r="B7">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1.655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>1.02</v>
+      </c>
+      <c r="C8">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>12.5</v>
+      </c>
+      <c r="B9">
+        <v>0.86</v>
+      </c>
+      <c r="C9">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="C10">
+        <v>2.6749999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>13.5</v>
+      </c>
+      <c r="B11">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="C11">
+        <v>3.0550000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906A053A-75C1-FF44-9971-89AB454196F5}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>2.7250000000000001</v>
+      </c>
+      <c r="C2">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.62698399999999999</v>
+      </c>
+      <c r="E2" s="10">
+        <v>12.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10.5</v>
+      </c>
+      <c r="B3">
+        <v>2.4049999999999998</v>
+      </c>
+      <c r="C3">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2.11</v>
+      </c>
+      <c r="C4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>11.5</v>
+      </c>
+      <c r="B5">
+        <v>1.84</v>
+      </c>
+      <c r="C5">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1.6</v>
+      </c>
+      <c r="C6">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>12.5</v>
+      </c>
+      <c r="B7">
+        <v>1.385</v>
+      </c>
+      <c r="C7">
+        <v>1.7949999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1.2</v>
+      </c>
+      <c r="C8">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>13.5</v>
+      </c>
+      <c r="B9">
+        <v>1.0349999999999999</v>
+      </c>
+      <c r="C9">
+        <v>2.4449999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>0.89</v>
+      </c>
+      <c r="C10">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14.5</v>
+      </c>
+      <c r="B11">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="C11">
+        <v>3.1749999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{857BD3D2-160D-134F-AA7B-6F51CA46B0CC}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>3.01</v>
+      </c>
+      <c r="C2">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
+        <v>0.75793650793650791</v>
+      </c>
+      <c r="E2">
+        <v>12.41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10.5</v>
+      </c>
+      <c r="B3">
+        <v>2.68</v>
+      </c>
+      <c r="C3">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2.38</v>
+      </c>
+      <c r="C4">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>11.5</v>
+      </c>
+      <c r="B5">
+        <v>2.105</v>
+      </c>
+      <c r="C5">
+        <v>1.1950000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1.86</v>
+      </c>
+      <c r="C6">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>12.5</v>
+      </c>
+      <c r="B7">
+        <v>1.635</v>
+      </c>
+      <c r="C7">
+        <v>1.7250000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1.44</v>
+      </c>
+      <c r="C8">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>13.5</v>
+      </c>
+      <c r="B9">
+        <v>1.27</v>
+      </c>
+      <c r="C9">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1.115</v>
+      </c>
+      <c r="C10">
+        <v>2.7050000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14.5</v>
+      </c>
+      <c r="B11">
+        <v>0.98</v>
+      </c>
+      <c r="C11">
+        <v>3.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>